<commit_message>
Update data for UI_MyPreference
</commit_message>
<xml_diff>
--- a/data/UI_MyPreference.xlsx
+++ b/data/UI_MyPreference.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="296">
   <si>
     <t>Please Select One</t>
   </si>
@@ -792,9 +792,6 @@
     <t>Recycling Fee</t>
   </si>
   <si>
-    <t>Request Addl %</t>
-  </si>
-  <si>
     <t>Request Net</t>
   </si>
   <si>
@@ -898,6 +895,15 @@
   </si>
   <si>
     <t>Total Requested Discount</t>
+  </si>
+  <si>
+    <t>Global List Price(USD)</t>
+  </si>
+  <si>
+    <t>Global Net Price(USD)</t>
+  </si>
+  <si>
+    <t>Request Total %</t>
   </si>
 </sst>
 </file>
@@ -1245,26 +1251,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C237"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="G48" sqref="G48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.140625" customWidth="1"/>
     <col min="2" max="2" width="29.85546875" customWidth="1"/>
-    <col min="3" max="3" width="26" customWidth="1"/>
+    <col min="3" max="3" width="27.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1272,7 +1278,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C2" t="s">
         <v>236</v>
@@ -1283,7 +1289,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C3" t="s">
         <v>237</v>
@@ -1294,10 +1300,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1305,7 +1311,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C5" t="s">
         <v>238</v>
@@ -1316,7 +1322,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C6" t="s">
         <v>239</v>
@@ -1367,7 +1373,7 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1375,7 +1381,7 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1383,7 +1389,7 @@
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1391,7 +1397,7 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>245</v>
+        <v>293</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1399,7 +1405,7 @@
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>246</v>
+        <v>294</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1407,7 +1413,7 @@
         <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1415,7 +1421,7 @@
         <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1423,7 +1429,7 @@
         <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1431,7 +1437,7 @@
         <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1439,7 +1445,7 @@
         <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>283</v>
+        <v>249</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1447,7 +1453,7 @@
         <v>20</v>
       </c>
       <c r="C22" t="s">
-        <v>284</v>
+        <v>250</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1455,7 +1461,7 @@
         <v>21</v>
       </c>
       <c r="C23" t="s">
-        <v>251</v>
+        <v>282</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -1463,7 +1469,7 @@
         <v>22</v>
       </c>
       <c r="C24" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -1471,7 +1477,7 @@
         <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>277</v>
+        <v>251</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -1479,7 +1485,7 @@
         <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>252</v>
+        <v>284</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1487,7 +1493,7 @@
         <v>25</v>
       </c>
       <c r="C27" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -1495,7 +1501,7 @@
         <v>26</v>
       </c>
       <c r="C28" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -1503,7 +1509,7 @@
         <v>27</v>
       </c>
       <c r="C29" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -1511,7 +1517,7 @@
         <v>28</v>
       </c>
       <c r="C30" t="s">
-        <v>288</v>
+        <v>253</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -1519,7 +1525,7 @@
         <v>29</v>
       </c>
       <c r="C31" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -1527,7 +1533,7 @@
         <v>30</v>
       </c>
       <c r="C32" t="s">
-        <v>254</v>
+        <v>287</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -1535,7 +1541,7 @@
         <v>31</v>
       </c>
       <c r="C33" t="s">
-        <v>255</v>
+        <v>288</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -1543,7 +1549,7 @@
         <v>32</v>
       </c>
       <c r="C34" t="s">
-        <v>290</v>
+        <v>254</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -1551,7 +1557,7 @@
         <v>33</v>
       </c>
       <c r="C35" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -1559,7 +1565,7 @@
         <v>34</v>
       </c>
       <c r="C36" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -1567,7 +1573,7 @@
         <v>35</v>
       </c>
       <c r="C37" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -1575,7 +1581,7 @@
         <v>36</v>
       </c>
       <c r="C38" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -1583,7 +1589,7 @@
         <v>37</v>
       </c>
       <c r="C39" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -1591,7 +1597,7 @@
         <v>38</v>
       </c>
       <c r="C40" t="s">
-        <v>259</v>
+        <v>291</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -1599,7 +1605,7 @@
         <v>39</v>
       </c>
       <c r="C41" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -1607,7 +1613,7 @@
         <v>40</v>
       </c>
       <c r="C42" t="s">
-        <v>261</v>
+        <v>295</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -1615,7 +1621,7 @@
         <v>41</v>
       </c>
       <c r="C43" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -1623,7 +1629,7 @@
         <v>42</v>
       </c>
       <c r="C44" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -1631,7 +1637,7 @@
         <v>43</v>
       </c>
       <c r="C45" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -1639,7 +1645,7 @@
         <v>44</v>
       </c>
       <c r="C46" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -1647,7 +1653,7 @@
         <v>45</v>
       </c>
       <c r="C47" t="s">
-        <v>278</v>
+        <v>263</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -1655,7 +1661,7 @@
         <v>46</v>
       </c>
       <c r="C48" t="s">
-        <v>293</v>
+        <v>264</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -1663,7 +1669,7 @@
         <v>47</v>
       </c>
       <c r="C49" t="s">
-        <v>266</v>
+        <v>277</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -1671,7 +1677,7 @@
         <v>48</v>
       </c>
       <c r="C50" t="s">
-        <v>267</v>
+        <v>292</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -1679,17 +1685,23 @@
         <v>49</v>
       </c>
       <c r="C51" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>50</v>
       </c>
+      <c r="C52" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>51</v>
+      </c>
+      <c r="C53" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>